<commit_message>
Fix one test. Write high level public method to be called by the user. Change infer_freq method
</commit_message>
<xml_diff>
--- a/tests/cases/test_case2.xlsx
+++ b/tests/cases/test_case2.xlsx
@@ -54,9 +54,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="188" formatCode="dd\-mm\-yy"/>
-    <numFmt numFmtId="189" formatCode="0.0000"/>
-    <numFmt numFmtId="191" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="mmmm\-yy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -471,124 +471,124 @@
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="188" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="189" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="191" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -901,8 +901,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:H2993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2187" workbookViewId="0">
+      <selection activeCell="F2194" sqref="F2194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.3" x14ac:dyDescent="0.25"/>
@@ -19169,7 +19169,7 @@
         <v>3.9817999999999998</v>
       </c>
       <c r="F2196" s="24">
-        <v>39783</v>
+        <v>40513</v>
       </c>
     </row>
     <row r="2197" spans="3:6" ht="15.95" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>